<commit_message>
Previous model cell isolation progress
</commit_message>
<xml_diff>
--- a/ephyz/ephyz-property-values-by-paper.xlsx
+++ b/ephyz/ephyz-property-values-by-paper.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$70</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$84</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="205">
   <si>
     <t>Paper</t>
   </si>
@@ -577,12 +577,6 @@
     <t>Fascilitation Time Constant</t>
   </si>
   <si>
-    <t>STD. Firing rate started slow then INCREASED to SS. Fascilitating</t>
-  </si>
-  <si>
-    <t>Mean increase of firing rate</t>
-  </si>
-  <si>
     <t>Rebound potentials</t>
   </si>
   <si>
@@ -644,6 +638,18 @@
   <si>
     <t>NMDA Receptor-Dependent Synaptic Activation of TRPC
 Channels in Olfactory Bulb Granule Cells</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>Intrinsic biophysical diversity decorrelates neuronal firing while increasing information content</t>
+  </si>
+  <si>
+    <t>STD. Firing rate started slow then INCREASED to SS. Fascilitating. Temp was "RT"</t>
+  </si>
+  <si>
+    <t>Mean increase of firing rate.  Temp was "RT"</t>
   </si>
 </sst>
 </file>
@@ -986,11 +992,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I84"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:J84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,12 +1006,13 @@
     <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="49" customWidth="1"/>
-    <col min="9" max="9" width="63.85546875" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="49" customWidth="1"/>
+    <col min="10" max="10" width="63.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1026,14 +1034,17 @@
       <c r="G1" t="s">
         <v>62</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>120</v>
       </c>
@@ -1049,11 +1060,11 @@
       <c r="E2" t="s">
         <v>134</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>122</v>
       </c>
@@ -1069,11 +1080,11 @@
       <c r="E3" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>124</v>
       </c>
@@ -1089,11 +1100,11 @@
       <c r="E4" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="J4" s="6" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>126</v>
       </c>
@@ -1109,11 +1120,11 @@
       <c r="E5" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="J5" s="6" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>126</v>
       </c>
@@ -1129,11 +1140,11 @@
       <c r="E6" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="J6" s="6" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>126</v>
       </c>
@@ -1149,11 +1160,11 @@
       <c r="E7" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="J7" s="6" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>84</v>
       </c>
@@ -1169,11 +1180,11 @@
       <c r="E8" t="s">
         <v>88</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>84</v>
       </c>
@@ -1189,11 +1200,11 @@
       <c r="E9" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>84</v>
       </c>
@@ -1209,11 +1220,11 @@
       <c r="E10" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>84</v>
       </c>
@@ -1229,11 +1240,11 @@
       <c r="E11" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>84</v>
       </c>
@@ -1249,11 +1260,11 @@
       <c r="E12" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>84</v>
       </c>
@@ -1269,11 +1280,11 @@
       <c r="E13" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>84</v>
       </c>
@@ -1289,11 +1300,11 @@
       <c r="E14" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>84</v>
       </c>
@@ -1309,11 +1320,11 @@
       <c r="E15" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>118</v>
       </c>
@@ -1332,14 +1343,17 @@
       <c r="F16" t="s">
         <v>116</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="6">
+        <v>36</v>
+      </c>
+      <c r="I16" t="s">
         <v>115</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>113</v>
       </c>
@@ -1358,11 +1372,14 @@
       <c r="F17" t="s">
         <v>111</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="6">
+        <v>37</v>
+      </c>
+      <c r="I17" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>113</v>
       </c>
@@ -1381,11 +1398,14 @@
       <c r="F18" t="s">
         <v>109</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="6">
+        <v>37</v>
+      </c>
+      <c r="I18" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>108</v>
       </c>
@@ -1404,11 +1424,14 @@
       <c r="F19" t="s">
         <v>106</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="6">
+        <v>35</v>
+      </c>
+      <c r="I19" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>104</v>
       </c>
@@ -1425,7 +1448,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>102</v>
       </c>
@@ -1441,11 +1464,11 @@
       <c r="E21" t="s">
         <v>119</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>99</v>
       </c>
@@ -1461,11 +1484,11 @@
       <c r="E22" t="s">
         <v>119</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>96</v>
       </c>
@@ -1484,14 +1507,17 @@
       <c r="F23" t="s">
         <v>93</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="H23" s="6">
+        <v>32</v>
+      </c>
+      <c r="I23" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="I23" s="5" t="s">
+      <c r="J23" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>96</v>
       </c>
@@ -1511,11 +1537,14 @@
         <f>"-5.2 +- 1.5 mV (n =  9)"</f>
         <v>-5.2 +- 1.5 mV (n =  9)</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="H24" s="6">
+        <v>32</v>
+      </c>
+      <c r="I24" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>96</v>
       </c>
@@ -1534,11 +1563,14 @@
       <c r="F25" t="s">
         <v>89</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="H25" s="6">
+        <v>32</v>
+      </c>
+      <c r="I25" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -1557,11 +1589,14 @@
       <c r="F26" t="s">
         <v>13</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" s="6">
+        <v>35</v>
+      </c>
+      <c r="I26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -1580,11 +1615,14 @@
       <c r="F27" t="s">
         <v>13</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27" s="6">
+        <v>35</v>
+      </c>
+      <c r="I27" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -1604,14 +1642,17 @@
         <v>31</v>
       </c>
       <c r="G28" s="1"/>
-      <c r="H28" t="s">
+      <c r="H28" s="6">
+        <v>35</v>
+      </c>
+      <c r="I28" t="s">
         <v>17</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -1631,11 +1672,14 @@
         <v>35</v>
       </c>
       <c r="G29" s="1"/>
-      <c r="H29" t="s">
+      <c r="H29" s="6">
+        <v>35</v>
+      </c>
+      <c r="I29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -1655,11 +1699,14 @@
         <v>36</v>
       </c>
       <c r="G30" s="1"/>
-      <c r="H30" t="s">
+      <c r="H30" s="6">
+        <v>35</v>
+      </c>
+      <c r="I30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -1679,11 +1726,14 @@
         <v>32</v>
       </c>
       <c r="G31" s="1"/>
-      <c r="H31" t="s">
+      <c r="H31" s="6">
+        <v>35</v>
+      </c>
+      <c r="I31" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -1703,12 +1753,15 @@
         <v>34</v>
       </c>
       <c r="G32" s="1"/>
-      <c r="H32" t="str">
+      <c r="H32" s="6">
+        <v>35</v>
+      </c>
+      <c r="I32" t="str">
         <f>"-50 pA current"</f>
         <v>-50 pA current</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -1728,11 +1781,14 @@
         <v>33</v>
       </c>
       <c r="G33" s="1"/>
-      <c r="H33" t="s">
+      <c r="H33" s="6">
+        <v>35</v>
+      </c>
+      <c r="I33" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -1752,11 +1808,14 @@
         <v>39</v>
       </c>
       <c r="G34" s="1"/>
-      <c r="H34" t="s">
+      <c r="H34" s="6">
+        <v>35</v>
+      </c>
+      <c r="I34" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -1776,8 +1835,11 @@
         <v>41</v>
       </c>
       <c r="G35" s="1"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H35" s="6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -1793,14 +1855,17 @@
       <c r="E36" t="s">
         <v>42</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H36" s="6">
+        <v>37</v>
+      </c>
+      <c r="I36" t="s">
         <v>45</v>
       </c>
-      <c r="I36" t="s">
+      <c r="J36" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -1816,11 +1881,14 @@
       <c r="E37" t="s">
         <v>43</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H37" s="6">
+        <v>37</v>
+      </c>
+      <c r="I37" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>8</v>
       </c>
@@ -1836,11 +1904,14 @@
       <c r="E38" t="s">
         <v>44</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H38" s="6">
+        <v>37</v>
+      </c>
+      <c r="I38" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -1862,14 +1933,17 @@
       <c r="G39">
         <v>35</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H39" s="6">
+        <v>37</v>
+      </c>
+      <c r="I39" t="s">
         <v>47</v>
       </c>
-      <c r="I39" s="2" t="s">
+      <c r="J39" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -1891,11 +1965,14 @@
       <c r="G40">
         <v>10</v>
       </c>
-      <c r="H40" t="s">
+      <c r="H40" s="6">
+        <v>37</v>
+      </c>
+      <c r="I40" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>8</v>
       </c>
@@ -1917,11 +1994,14 @@
       <c r="G41">
         <v>10</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H41" s="6">
+        <v>37</v>
+      </c>
+      <c r="I41" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>8</v>
       </c>
@@ -1943,11 +2023,14 @@
       <c r="G42">
         <v>10</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H42" s="6">
+        <v>37</v>
+      </c>
+      <c r="I42" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>8</v>
       </c>
@@ -1969,11 +2052,14 @@
       <c r="G43">
         <v>10</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H43" s="6">
+        <v>37</v>
+      </c>
+      <c r="I43" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>8</v>
       </c>
@@ -1995,11 +2081,14 @@
       <c r="G44">
         <v>10</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H44" s="6">
+        <v>37</v>
+      </c>
+      <c r="I44" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -2021,11 +2110,14 @@
       <c r="G45">
         <v>10</v>
       </c>
-      <c r="H45" t="s">
+      <c r="H45" s="6">
+        <v>37</v>
+      </c>
+      <c r="I45" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>8</v>
       </c>
@@ -2047,11 +2139,14 @@
       <c r="G46">
         <v>35</v>
       </c>
-      <c r="H46" t="s">
+      <c r="H46" s="6">
+        <v>37</v>
+      </c>
+      <c r="I46" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>8</v>
       </c>
@@ -2073,11 +2168,14 @@
       <c r="G47">
         <v>35</v>
       </c>
-      <c r="H47" t="s">
+      <c r="H47" s="6">
+        <v>37</v>
+      </c>
+      <c r="I47" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>8</v>
       </c>
@@ -2099,8 +2197,11 @@
       <c r="G48">
         <v>12</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H48" s="6">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>8</v>
       </c>
@@ -2122,8 +2223,11 @@
       <c r="G49">
         <v>12</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H49" s="6">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>8</v>
       </c>
@@ -2145,8 +2249,11 @@
       <c r="G50">
         <v>12</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H50" s="6">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>8</v>
       </c>
@@ -2168,8 +2275,11 @@
       <c r="G51">
         <v>12</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H51" s="6">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>8</v>
       </c>
@@ -2191,8 +2301,11 @@
       <c r="G52">
         <v>12</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H52" s="6">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>8</v>
       </c>
@@ -2214,8 +2327,11 @@
       <c r="G53">
         <v>12</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H53" s="6">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>8</v>
       </c>
@@ -2237,8 +2353,11 @@
       <c r="G54">
         <v>28</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H54" s="6">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>8</v>
       </c>
@@ -2260,8 +2379,11 @@
       <c r="G55">
         <v>28</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H55" s="6">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>8</v>
       </c>
@@ -2283,14 +2405,17 @@
       <c r="G56" s="6">
         <v>28</v>
       </c>
-      <c r="H56" s="6" t="s">
+      <c r="H56" s="6">
+        <v>37</v>
+      </c>
+      <c r="I56" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="I56" s="7" t="s">
+      <c r="J56" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>8</v>
       </c>
@@ -2306,11 +2431,14 @@
       <c r="E57" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="I57" s="4" t="s">
+      <c r="H57" s="6">
+        <v>37</v>
+      </c>
+      <c r="J57" s="4" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="58" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>8</v>
       </c>
@@ -2326,11 +2454,14 @@
       <c r="E58" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="I58" s="4" t="s">
+      <c r="H58" s="6">
+        <v>37</v>
+      </c>
+      <c r="J58" s="4" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>78</v>
       </c>
@@ -2346,14 +2477,17 @@
       <c r="E59" t="s">
         <v>80</v>
       </c>
-      <c r="H59" s="3" t="s">
+      <c r="H59" s="6">
+        <v>30</v>
+      </c>
+      <c r="I59" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="I59" s="2" t="s">
+      <c r="J59" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>78</v>
       </c>
@@ -2369,14 +2503,17 @@
       <c r="E60" t="s">
         <v>16</v>
       </c>
-      <c r="H60" s="3" t="s">
+      <c r="H60" s="6">
+        <v>30</v>
+      </c>
+      <c r="I60" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="I60" t="s">
+      <c r="J60" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>143</v>
       </c>
@@ -2393,7 +2530,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>146</v>
       </c>
@@ -2410,7 +2547,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>120</v>
       </c>
@@ -2427,7 +2564,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>122</v>
       </c>
@@ -2444,7 +2581,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>148</v>
       </c>
@@ -2461,7 +2598,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>126</v>
       </c>
@@ -2478,10 +2615,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>150</v>
       </c>
+      <c r="B67" t="s">
+        <v>202</v>
+      </c>
       <c r="C67" t="s">
         <v>7</v>
       </c>
@@ -2497,14 +2637,17 @@
       <c r="G67">
         <v>34</v>
       </c>
-      <c r="H67" t="s">
+      <c r="H67" s="6">
+        <v>35</v>
+      </c>
+      <c r="I67" t="s">
         <v>153</v>
       </c>
-      <c r="I67" t="s">
+      <c r="J67" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>104</v>
       </c>
@@ -2521,7 +2664,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>154</v>
       </c>
@@ -2538,7 +2681,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>159</v>
       </c>
@@ -2554,14 +2697,17 @@
       <c r="E70" t="s">
         <v>157</v>
       </c>
-      <c r="H70" t="s">
+      <c r="H70" s="6">
+        <v>33</v>
+      </c>
+      <c r="I70" t="s">
         <v>156</v>
       </c>
-      <c r="I70" s="7" t="s">
+      <c r="J70" s="7" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
         <v>159</v>
       </c>
@@ -2580,8 +2726,11 @@
       <c r="F71" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H71" s="6">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
         <v>159</v>
       </c>
@@ -2600,8 +2749,11 @@
       <c r="F72" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H72" s="6">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
         <v>159</v>
       </c>
@@ -2614,8 +2766,11 @@
       <c r="D73" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H73" s="6">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>166</v>
       </c>
@@ -2631,11 +2786,14 @@
       <c r="E74" t="s">
         <v>167</v>
       </c>
-      <c r="I74" t="s">
+      <c r="H74" s="6">
+        <v>37</v>
+      </c>
+      <c r="J74" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
         <v>166</v>
       </c>
@@ -2651,11 +2809,14 @@
       <c r="E75" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="I75" s="6" t="s">
+      <c r="H75" s="6">
+        <v>37</v>
+      </c>
+      <c r="J75" s="6" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>174</v>
       </c>
@@ -2677,14 +2838,17 @@
       <c r="G76">
         <v>35</v>
       </c>
-      <c r="H76" t="s">
+      <c r="H76" s="6">
+        <v>22</v>
+      </c>
+      <c r="I76" t="s">
         <v>179</v>
       </c>
-      <c r="I76" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J76" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
         <v>174</v>
       </c>
@@ -2706,11 +2870,14 @@
       <c r="G77">
         <v>35</v>
       </c>
-      <c r="I77" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H77" s="6">
+        <v>22</v>
+      </c>
+      <c r="J77" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>154</v>
       </c>
@@ -2727,7 +2894,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
         <v>8</v>
       </c>
@@ -2741,16 +2908,19 @@
         <v>11</v>
       </c>
       <c r="E79" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F79" t="s">
-        <v>184</v>
-      </c>
-      <c r="I79" s="6" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+      <c r="H79" s="6">
+        <v>37</v>
+      </c>
+      <c r="J79" s="6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
         <v>8</v>
       </c>
@@ -2764,48 +2934,54 @@
         <v>12</v>
       </c>
       <c r="E80" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="F80" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="F80" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="I80" t="s">
+      <c r="H80" s="6">
+        <v>37</v>
+      </c>
+      <c r="J80" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="B81" t="s">
+        <v>187</v>
+      </c>
+      <c r="C81" t="s">
+        <v>7</v>
+      </c>
+      <c r="D81" t="s">
+        <v>11</v>
+      </c>
+      <c r="E81" t="s">
+        <v>181</v>
+      </c>
+      <c r="F81" t="s">
+        <v>183</v>
+      </c>
+      <c r="H81" s="6">
+        <v>35</v>
+      </c>
+      <c r="I81" t="s">
         <v>188</v>
       </c>
-      <c r="B81" t="s">
+      <c r="J81" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>189</v>
       </c>
-      <c r="C81" t="s">
-        <v>7</v>
-      </c>
-      <c r="D81" t="s">
-        <v>11</v>
-      </c>
-      <c r="E81" t="s">
-        <v>183</v>
-      </c>
-      <c r="F81" t="s">
-        <v>185</v>
-      </c>
-      <c r="H81" t="s">
+      <c r="B82" t="s">
         <v>190</v>
       </c>
-      <c r="I81" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>191</v>
-      </c>
-      <c r="B82" t="s">
-        <v>192</v>
-      </c>
       <c r="C82" s="6" t="s">
         <v>7</v>
       </c>
@@ -2813,18 +2989,21 @@
         <v>11</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F82" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+      <c r="H82" s="6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C83" s="6" t="s">
         <v>7</v>
@@ -2833,27 +3012,30 @@
         <v>94</v>
       </c>
       <c r="E83" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F83" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G83">
         <v>49</v>
       </c>
-      <c r="H83" t="s">
+      <c r="H83" s="6">
+        <v>21</v>
+      </c>
+      <c r="I83" t="s">
+        <v>198</v>
+      </c>
+      <c r="J83" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="B84" s="5" t="s">
         <v>200</v>
-      </c>
-      <c r="I83" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="B84" s="5" t="s">
-        <v>202</v>
       </c>
       <c r="C84" s="6" t="s">
         <v>7</v>
@@ -2862,22 +3044,32 @@
         <v>94</v>
       </c>
       <c r="E84" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F84" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G84">
         <v>49</v>
       </c>
-      <c r="H84" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="I84" s="5" t="s">
-        <v>199</v>
+      <c r="H84" s="6">
+        <v>21</v>
+      </c>
+      <c r="I84" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="J84" s="5" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J84">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Mice"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
All ephyz unit tests and data in DB
</commit_message>
<xml_diff>
--- a/ephyz/ephyz-property-values-by-paper.xlsx
+++ b/ephyz/ephyz-property-values-by-paper.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$78</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$D$19</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="181">
   <si>
     <t>Paper</t>
   </si>
@@ -325,9 +326,6 @@
     <t>Corrected</t>
   </si>
   <si>
-    <t>Corrected 14mv</t>
-  </si>
-  <si>
     <t>NOT corrected 13mV</t>
   </si>
   <si>
@@ -335,12 +333,6 @@
   </si>
   <si>
     <t>not REPORTED</t>
-  </si>
-  <si>
-    <t>NOT corrected 9.5V</t>
-  </si>
-  <si>
-    <t>Vrest Corrected 14mV</t>
   </si>
   <si>
     <t>4s of -300pA into soma</t>
@@ -962,9 +954,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I1" activeCellId="1" sqref="A1:A1048576 I1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
@@ -1008,7 +1000,7 @@
         <v>43</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>90</v>
@@ -1052,7 +1044,7 @@
         <v>37</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L2" t="s">
         <v>38</v>
@@ -1078,14 +1070,14 @@
         <v>46</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H3" s="4"/>
       <c r="J3" s="4">
         <v>35</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L3" t="s">
         <v>17</v>
@@ -1111,14 +1103,14 @@
         <v>47</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H4" s="4"/>
       <c r="J4" s="4">
         <v>35</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L4" t="s">
         <v>14</v>
@@ -1126,10 +1118,10 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>6</v>
@@ -1138,13 +1130,13 @@
         <v>57</v>
       </c>
       <c r="E5" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F5" s="4">
         <v>32</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4" t="s">
@@ -1154,10 +1146,10 @@
         <v>32</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="M5" s="4"/>
     </row>
@@ -1190,7 +1182,7 @@
         <v>37</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L6" s="4" t="s">
         <v>40</v>
@@ -1210,7 +1202,7 @@
         <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F7" s="4">
         <v>767</v>
@@ -1228,7 +1220,7 @@
         <v>37</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L7" t="s">
         <v>34</v>
@@ -1248,7 +1240,7 @@
         <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F8" s="4">
         <v>53</v>
@@ -1264,7 +1256,7 @@
         <v>35</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L8" t="s">
         <v>26</v>
@@ -1284,7 +1276,7 @@
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F9" s="4">
         <v>55</v>
@@ -1300,7 +1292,7 @@
         <v>35</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1335,7 +1327,7 @@
         <v>37</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L10" t="s">
         <v>33</v>
@@ -1371,7 +1363,7 @@
         <v>35</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L11" t="s">
         <v>12</v>
@@ -1394,13 +1386,13 @@
         <v>9</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F12" s="4">
         <v>762</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H12" s="4">
         <v>12</v>
@@ -1412,7 +1404,7 @@
         <v>37</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -1435,7 +1427,7 @@
         <v>763</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H13" s="4">
         <v>12</v>
@@ -1447,7 +1439,7 @@
         <v>37</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L13" t="s">
         <v>95</v>
@@ -1485,7 +1477,7 @@
         <v>37</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L14" t="s">
         <v>36</v>
@@ -1511,7 +1503,7 @@
         <v>764</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H15">
         <v>12</v>
@@ -1523,7 +1515,7 @@
         <v>37</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1546,7 +1538,7 @@
         <v>54</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="4" t="s">
@@ -1556,7 +1548,7 @@
         <v>35</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M16" s="4"/>
     </row>
@@ -1574,13 +1566,13 @@
         <v>9</v>
       </c>
       <c r="E17" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F17" s="4">
         <v>77</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H17" s="4">
         <v>28</v>
@@ -1592,7 +1584,7 @@
         <v>37</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1609,13 +1601,13 @@
         <v>8</v>
       </c>
       <c r="E18" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F18" s="4">
         <v>57</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="H18" s="4">
         <v>35</v>
@@ -1627,7 +1619,7 @@
         <v>37</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -1644,13 +1636,13 @@
         <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F19" s="4">
         <v>48</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="4" t="s">
@@ -1660,7 +1652,7 @@
         <v>35</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M19" s="4"/>
     </row>
@@ -1684,7 +1676,7 @@
         <v>746</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H20">
         <v>35</v>
@@ -1693,7 +1685,7 @@
         <v>37</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L20" s="4" t="s">
         <v>31</v>
@@ -1732,10 +1724,10 @@
         <v>37</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>75</v>
@@ -1761,7 +1753,7 @@
         <v>78</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H22" s="4">
         <v>28</v>
@@ -1773,7 +1765,7 @@
         <v>37</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -1805,10 +1797,10 @@
         <v>22</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="M23" s="4" t="s">
         <v>92</v>
@@ -1828,13 +1820,13 @@
         <v>8</v>
       </c>
       <c r="E24" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F24" s="4">
         <v>751</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H24" s="4">
         <v>35</v>
@@ -1843,10 +1835,10 @@
         <v>37</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="M24" s="2" t="s">
         <v>75</v>
@@ -1866,13 +1858,13 @@
         <v>9</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F25" s="4">
         <v>80</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H25" s="4">
         <v>26</v>
@@ -1884,7 +1876,7 @@
         <v>37</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M25" s="4"/>
     </row>
@@ -1902,7 +1894,7 @@
         <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F26" s="4">
         <v>753</v>
@@ -1917,7 +1909,7 @@
         <v>22</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L26" t="s">
         <v>81</v>
@@ -1928,10 +1920,10 @@
     </row>
     <row r="27" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>6</v>
@@ -1946,7 +1938,7 @@
         <v>63</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H27" s="4">
         <v>29</v>
@@ -1958,7 +1950,7 @@
         <v>24.5</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="M27" s="4"/>
     </row>
@@ -1991,7 +1983,7 @@
         <v>37</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M28" s="4"/>
     </row>
@@ -2015,7 +2007,7 @@
         <v>58</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H29">
         <v>35</v>
@@ -2027,7 +2019,7 @@
         <v>37</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L29" t="s">
         <v>29</v>
@@ -2062,16 +2054,16 @@
         <v>37</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M30" s="4"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>6</v>
@@ -2086,16 +2078,16 @@
         <v>72</v>
       </c>
       <c r="G31" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="J31" s="4">
         <v>33.5</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -2112,13 +2104,13 @@
         <v>9</v>
       </c>
       <c r="E32" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F32" s="4">
         <v>765</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H32" s="4">
         <v>28</v>
@@ -2130,16 +2122,16 @@
         <v>37</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M32" s="4"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>6</v>
@@ -2154,19 +2146,19 @@
         <v>73</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H33" s="4">
         <v>3</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="J33" s="4">
         <v>36</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="L33" s="4"/>
     </row>
@@ -2190,7 +2182,7 @@
         <v>79</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H34" s="4">
         <v>28</v>
@@ -2202,15 +2194,15 @@
         <v>37</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>6</v>
@@ -2225,7 +2217,7 @@
         <v>34</v>
       </c>
       <c r="G35" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="I35" s="4" t="s">
         <v>21</v>
@@ -2234,18 +2226,18 @@
         <v>32</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C36" t="s">
         <v>6</v>
@@ -2260,7 +2252,7 @@
         <v>33</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I36" s="4" t="s">
         <v>21</v>
@@ -2269,18 +2261,18 @@
         <v>32</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L36" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="37" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>6</v>
@@ -2289,13 +2281,13 @@
         <v>57</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F37" s="4">
         <v>28</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="I37" s="4" t="s">
         <v>21</v>
@@ -2304,18 +2296,18 @@
         <v>32</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>6</v>
@@ -2330,7 +2322,7 @@
         <v>29</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H38" s="4"/>
       <c r="I38" s="4" t="s">
@@ -2340,18 +2332,18 @@
         <v>32</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L38" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="39" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>6</v>
@@ -2360,13 +2352,13 @@
         <v>57</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F39" s="4">
         <v>31</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="I39" s="4" t="s">
         <v>21</v>
@@ -2375,18 +2367,18 @@
         <v>32</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="40" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>6</v>
@@ -2395,13 +2387,13 @@
         <v>57</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F40" s="4">
         <v>36</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="I40" s="4" t="s">
         <v>21</v>
@@ -2410,10 +2402,10 @@
         <v>32</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L40" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="41" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2436,7 +2428,7 @@
         <v>747</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="H41" s="4">
         <v>28</v>
@@ -2445,7 +2437,7 @@
         <v>37</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L41" s="4" t="s">
         <v>31</v>
@@ -2485,10 +2477,10 @@
         <v>37</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L42" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="M42" s="2" t="s">
         <v>75</v>
@@ -2508,13 +2500,13 @@
         <v>9</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F43" s="4">
         <v>752</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H43" s="4">
         <v>28</v>
@@ -2523,10 +2515,10 @@
         <v>37</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L43" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="M43" s="2" t="s">
         <v>75</v>
@@ -2534,10 +2526,10 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C44" t="s">
         <v>6</v>
@@ -2552,7 +2544,7 @@
         <v>30</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I44" s="4" t="s">
         <v>21</v>
@@ -2561,18 +2553,18 @@
         <v>32</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L44" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="45" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>6</v>
@@ -2587,7 +2579,7 @@
         <v>35</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H45" s="4">
         <v>30</v>
@@ -2596,7 +2588,7 @@
         <v>32</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="L45" s="4" t="s">
         <v>31</v>
@@ -2628,7 +2620,7 @@
         <v>32</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L46" s="3" t="s">
         <v>55</v>
@@ -2639,10 +2631,10 @@
     </row>
     <row r="47" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>6</v>
@@ -2657,7 +2649,7 @@
         <v>64</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="I47" s="4" t="s">
         <v>21</v>
@@ -2666,15 +2658,15 @@
         <v>35</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>6</v>
@@ -2689,17 +2681,17 @@
         <v>66</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H48" s="4"/>
       <c r="I48" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="J48" s="4">
         <v>22</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
@@ -2732,7 +2724,7 @@
         <v>35</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L49" t="str">
         <f>"-50 pA current"</f>
@@ -2759,7 +2751,7 @@
         <v>68</v>
       </c>
       <c r="G50" s="9" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H50" s="4"/>
       <c r="I50" s="4" t="s">
@@ -2769,7 +2761,7 @@
         <v>22</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
@@ -2799,7 +2791,7 @@
         <v>37</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L51" t="s">
         <v>93</v>
@@ -2810,10 +2802,10 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>6</v>
@@ -2828,27 +2820,27 @@
         <v>75</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H52" s="4">
         <v>6</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="J52" s="4">
         <v>36</v>
       </c>
       <c r="K52" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>6</v>
@@ -2857,13 +2849,13 @@
         <v>8</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F53" s="4">
         <v>62</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H53" s="4">
         <v>29</v>
@@ -2875,7 +2867,7 @@
         <v>24.5</v>
       </c>
       <c r="K53" s="6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
@@ -2907,7 +2899,7 @@
         <v>35</v>
       </c>
       <c r="K54" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L54" t="s">
         <v>16</v>
@@ -2942,10 +2934,10 @@
         <v>37</v>
       </c>
       <c r="K55" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L55" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="56" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2977,10 +2969,10 @@
         <v>37</v>
       </c>
       <c r="K56" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L56" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="57" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -3009,7 +3001,7 @@
         <v>37</v>
       </c>
       <c r="K57" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L57" s="4" t="s">
         <v>93</v>
@@ -3020,10 +3012,10 @@
     </row>
     <row r="58" spans="1:13" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>6</v>
@@ -3032,24 +3024,24 @@
         <v>57</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F58" s="4">
         <v>757</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H58" s="4">
         <v>77</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="59" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>89</v>
@@ -3067,7 +3059,7 @@
         <v>40</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H59" s="4">
         <v>20</v>
@@ -3079,7 +3071,7 @@
         <v>21</v>
       </c>
       <c r="K59" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
@@ -3112,7 +3104,7 @@
         <v>96</v>
       </c>
       <c r="L60" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
@@ -3129,7 +3121,7 @@
         <v>8</v>
       </c>
       <c r="E61" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F61" s="4">
         <v>60</v>
@@ -3148,15 +3140,15 @@
         <v>37</v>
       </c>
       <c r="K61" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>6</v>
@@ -3165,23 +3157,23 @@
         <v>8</v>
       </c>
       <c r="E62" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F62" s="4">
         <v>67</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H62" s="4"/>
       <c r="I62" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="J62" s="4">
         <v>22</v>
       </c>
       <c r="K62" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
@@ -3198,13 +3190,13 @@
         <v>8</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F63" s="4">
         <v>51</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H63" s="1"/>
       <c r="I63" s="4" t="s">
@@ -3214,12 +3206,12 @@
         <v>35</v>
       </c>
       <c r="K63" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>89</v>
@@ -3231,7 +3223,7 @@
         <v>57</v>
       </c>
       <c r="E64" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F64" s="4">
         <v>41</v>
@@ -3250,7 +3242,7 @@
         <v>21</v>
       </c>
       <c r="K64" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
@@ -3267,13 +3259,13 @@
         <v>8</v>
       </c>
       <c r="E65" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F65" s="4">
         <v>769</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H65" s="4">
         <v>35</v>
@@ -3285,7 +3277,7 @@
         <v>37</v>
       </c>
       <c r="K65" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
@@ -3302,13 +3294,13 @@
         <v>9</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F66" s="4">
         <v>760</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H66">
         <v>21</v>
@@ -3317,7 +3309,7 @@
         <v>37</v>
       </c>
       <c r="K66" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
@@ -3347,7 +3339,7 @@
         <v>36</v>
       </c>
       <c r="K67" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L67" t="s">
         <v>70</v>
@@ -3383,7 +3375,7 @@
         <v>32</v>
       </c>
       <c r="K68" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L68" s="3" t="s">
         <v>55</v>
@@ -3391,10 +3383,10 @@
     </row>
     <row r="69" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B69" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>6</v>
@@ -3403,25 +3395,25 @@
         <v>9</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F69" s="4">
         <v>761</v>
       </c>
       <c r="G69" s="10" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H69">
         <v>6</v>
       </c>
       <c r="I69" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="J69" s="4">
         <v>36</v>
       </c>
       <c r="K69" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
@@ -3451,7 +3443,7 @@
         <v>35</v>
       </c>
       <c r="K70" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L70" t="s">
         <v>60</v>
@@ -3484,7 +3476,7 @@
         <v>37</v>
       </c>
       <c r="K71" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L71" t="s">
         <v>65</v>
@@ -3516,7 +3508,7 @@
         <v>37</v>
       </c>
       <c r="K72" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L72" t="s">
         <v>65</v>
@@ -3536,13 +3528,13 @@
         <v>8</v>
       </c>
       <c r="E73" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F73" s="4">
         <v>758</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H73" s="4">
         <v>30</v>
@@ -3551,16 +3543,16 @@
         <v>37</v>
       </c>
       <c r="K73" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L73" s="4"/>
     </row>
     <row r="74" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>6</v>
@@ -3569,25 +3561,25 @@
         <v>8</v>
       </c>
       <c r="E74" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F74" s="4">
         <v>759</v>
       </c>
       <c r="G74" s="10" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H74" s="4">
         <v>7</v>
       </c>
       <c r="I74" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="J74" s="4">
         <v>36</v>
       </c>
       <c r="K74" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="L74" s="4"/>
     </row>
@@ -3611,7 +3603,7 @@
         <v>59</v>
       </c>
       <c r="G75" s="9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H75" s="4">
         <v>35</v>
@@ -3623,7 +3615,7 @@
         <v>37</v>
       </c>
       <c r="K75" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L75" s="4" t="s">
         <v>29</v>
@@ -3634,10 +3626,10 @@
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>6</v>
@@ -3652,7 +3644,7 @@
         <v>65</v>
       </c>
       <c r="G76" s="9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H76" s="4">
         <v>5</v>
@@ -3664,7 +3656,7 @@
         <v>35</v>
       </c>
       <c r="K76" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L76" s="4"/>
     </row>
@@ -3700,7 +3692,7 @@
         <v>35</v>
       </c>
       <c r="K77" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L77" s="4" t="s">
         <v>20</v>
@@ -3726,7 +3718,7 @@
         <v>69</v>
       </c>
       <c r="G78" s="9" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H78">
         <v>35</v>
@@ -3738,7 +3730,7 @@
         <v>22</v>
       </c>
       <c r="K78" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L78" s="4"/>
     </row>
@@ -3766,39 +3758,397 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A2:D78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="4" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4"/>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+    <row r="2" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D2" s="6"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20"/>
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22"/>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23"/>
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24"/>
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25"/>
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26"/>
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27"/>
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28"/>
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29"/>
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30"/>
+      <c r="B30"/>
+      <c r="C30"/>
+      <c r="D30"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31"/>
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32"/>
+      <c r="B32"/>
+      <c r="C32"/>
+      <c r="D32"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33"/>
+      <c r="B33"/>
+      <c r="C33"/>
+      <c r="D33"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34"/>
+      <c r="B34"/>
+      <c r="C34"/>
+      <c r="D34"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35"/>
+      <c r="B35"/>
+      <c r="C35"/>
+      <c r="D35"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36"/>
+      <c r="B36"/>
+      <c r="C36"/>
+      <c r="D36"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37"/>
+      <c r="B37"/>
+      <c r="C37"/>
+      <c r="D37"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38"/>
+      <c r="B38"/>
+      <c r="C38"/>
+      <c r="D38"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39"/>
+      <c r="B39"/>
+      <c r="C39"/>
+      <c r="D39"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40"/>
+      <c r="B40"/>
+      <c r="C40"/>
+      <c r="D40"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41"/>
+      <c r="B41"/>
+      <c r="C41"/>
+      <c r="D41"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42"/>
+      <c r="B42"/>
+      <c r="C42"/>
+      <c r="D42"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43"/>
+      <c r="B43"/>
+      <c r="C43"/>
+      <c r="D43"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44"/>
+      <c r="B44"/>
+      <c r="C44"/>
+      <c r="D44"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45"/>
+      <c r="B45"/>
+      <c r="C45"/>
+      <c r="D45"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46"/>
+      <c r="B46"/>
+      <c r="C46"/>
+      <c r="D46"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47"/>
+      <c r="B47"/>
+      <c r="C47"/>
+      <c r="D47"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48"/>
+      <c r="B48"/>
+      <c r="C48"/>
+      <c r="D48"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49"/>
+      <c r="B49"/>
+      <c r="C49"/>
+      <c r="D49"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50"/>
+      <c r="B50"/>
+      <c r="C50"/>
+      <c r="D50"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51"/>
+      <c r="B51"/>
+      <c r="C51"/>
+      <c r="D51"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52"/>
+      <c r="B52"/>
+      <c r="C52"/>
+      <c r="D52"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53"/>
+      <c r="B53"/>
+      <c r="C53"/>
+      <c r="D53"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54"/>
+      <c r="B54"/>
+      <c r="C54"/>
+      <c r="D54"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55"/>
+      <c r="B55"/>
+      <c r="C55"/>
+      <c r="D55"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56"/>
+      <c r="B56"/>
+      <c r="C56"/>
+      <c r="D56"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57"/>
+      <c r="B57"/>
+      <c r="C57"/>
+      <c r="D57"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58"/>
+      <c r="B58"/>
+      <c r="C58"/>
+      <c r="D58"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59"/>
+      <c r="B59"/>
+      <c r="C59"/>
+      <c r="D59"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60"/>
+      <c r="B60"/>
+      <c r="C60"/>
+      <c r="D60"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61"/>
+      <c r="B61"/>
+      <c r="C61"/>
+      <c r="D61"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62"/>
+      <c r="B62"/>
+      <c r="C62"/>
+      <c r="D62"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63"/>
+      <c r="B63"/>
+      <c r="C63"/>
+      <c r="D63"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64"/>
+      <c r="B64"/>
+      <c r="C64"/>
+      <c r="D64"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65"/>
+      <c r="B65"/>
+      <c r="C65"/>
+      <c r="D65"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66"/>
+      <c r="B66"/>
+      <c r="C66"/>
+      <c r="D66"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67"/>
+      <c r="B67"/>
+      <c r="C67"/>
+      <c r="D67"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68"/>
+      <c r="B68"/>
+      <c r="C68"/>
+      <c r="D68"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69"/>
+      <c r="B69"/>
+      <c r="C69"/>
+      <c r="D69"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70"/>
+      <c r="B70"/>
+      <c r="C70"/>
+      <c r="D70"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71"/>
+      <c r="B71"/>
+      <c r="C71"/>
+      <c r="D71"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72"/>
+      <c r="B72"/>
+      <c r="C72"/>
+      <c r="D72"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73"/>
+      <c r="B73"/>
+      <c r="C73"/>
+      <c r="D73"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74"/>
+      <c r="B74"/>
+      <c r="C74"/>
+      <c r="D74"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75"/>
+      <c r="B75"/>
+      <c r="C75"/>
+      <c r="D75"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76"/>
+      <c r="B76"/>
+      <c r="C76"/>
+      <c r="D76"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77"/>
+      <c r="B77"/>
+      <c r="C77"/>
+      <c r="D77"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78"/>
+      <c r="B78"/>
+      <c r="C78"/>
+      <c r="D78"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>